<commit_message>
commit with import actioncard from excel
</commit_message>
<xml_diff>
--- a/drugs_listt.xlsx
+++ b/drugs_listt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
   <si>
     <t>Index</t>
   </si>
@@ -43,6 +43,9 @@
     <t>Calcium Gluconate</t>
   </si>
   <si>
+    <t>Calpol500</t>
+  </si>
+  <si>
     <t>Cefazolin</t>
   </si>
   <si>
@@ -94,12 +97,6 @@
     <t>Dicloxacillin</t>
   </si>
   <si>
-    <t>Dolo</t>
-  </si>
-  <si>
-    <t>Dolo650</t>
-  </si>
-  <si>
     <t>Ergometrine</t>
   </si>
   <si>
@@ -163,6 +160,9 @@
     <t>Paracetamol</t>
   </si>
   <si>
+    <t>Paracetamol500</t>
+  </si>
+  <si>
     <t>Penicillin G (Benzylpenicillin)</t>
   </si>
   <si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Quinine</t>
+  </si>
+  <si>
+    <t>Safi</t>
   </si>
   <si>
     <t>Syntometrine</t>
@@ -585,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B65"/>
+  <dimension ref="A1:B67"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -989,7 +992,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,7 +1000,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1005,7 +1008,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1013,7 +1016,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,7 +1024,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1029,7 +1032,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1037,7 +1040,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1045,7 +1048,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1053,7 +1056,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1061,7 +1064,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1069,7 +1072,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1077,7 +1080,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,7 +1088,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1093,7 +1096,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1101,7 +1104,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,7 +1112,23 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
         <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit with module score and langId on card
</commit_message>
<xml_diff>
--- a/drugs_listt.xlsx
+++ b/drugs_listt.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Index</t>
   </si>
@@ -103,6 +103,9 @@
     <t>Erythromycin</t>
   </si>
   <si>
+    <t>Flaxon 650</t>
+  </si>
+  <si>
     <t>Flucloxacillin</t>
   </si>
   <si>
@@ -212,6 +215,9 @@
   </si>
   <si>
     <t>Vitamin X</t>
+  </si>
+  <si>
+    <t>flaxon 650</t>
   </si>
 </sst>
 </file>
@@ -588,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B70"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -992,7 +998,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -1008,7 +1014,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1016,7 +1022,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -1024,7 +1030,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -1032,7 +1038,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -1040,7 +1046,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,7 +1054,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -1056,7 +1062,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -1064,7 +1070,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -1072,7 +1078,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -1080,7 +1086,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -1088,7 +1094,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -1096,7 +1102,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -1104,7 +1110,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -1112,7 +1118,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,7 +1126,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -1128,7 +1134,31 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>